<commit_message>
Added few change in input dataset format
</commit_message>
<xml_diff>
--- a/Dataset/Open_Source_Dataset/Table_3.2.1.1.xlsx
+++ b/Dataset/Open_Source_Dataset/Table_3.2.1.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
   <si>
     <t>H2</t>
   </si>
@@ -41,12 +41,6 @@
   </si>
   <si>
     <t>D2</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
   </si>
   <si>
     <t>T3</t>
@@ -397,9 +391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -422,24 +414,12 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -458,26 +438,14 @@
         <v>1.5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -496,26 +464,14 @@
         <v>8.52</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -534,26 +490,14 @@
         <v>27.72</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -572,26 +516,14 @@
         <v>2.71</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -610,25 +542,7 @@
         <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -648,25 +562,7 @@
         <v>6303</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -686,25 +582,7 @@
         <v>145</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -724,25 +602,7 @@
         <v>330</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -762,25 +622,7 @@
         <v>129</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -802,24 +644,6 @@
       <c r="F11" t="s">
         <v>7</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -840,24 +664,6 @@
       <c r="F12" t="s">
         <v>7</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -878,24 +684,6 @@
       <c r="F13" t="s">
         <v>7</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -916,24 +704,6 @@
       <c r="F14" t="s">
         <v>7</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -954,24 +724,6 @@
       <c r="F15" t="s">
         <v>7</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -992,26 +744,8 @@
       <c r="F16" t="s">
         <v>8</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>117</v>
       </c>
@@ -1030,26 +764,8 @@
       <c r="F17" t="s">
         <v>8</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>421</v>
       </c>
@@ -1068,26 +784,8 @@
       <c r="F18" t="s">
         <v>8</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>71.599999999999994</v>
       </c>
@@ -1106,26 +804,8 @@
       <c r="F19" t="s">
         <v>8</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>730</v>
       </c>
@@ -1144,26 +824,8 @@
       <c r="F20" t="s">
         <v>8</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>43</v>
       </c>
@@ -1182,26 +844,8 @@
       <c r="F21" t="s">
         <v>8</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>100</v>
       </c>
@@ -1220,26 +864,8 @@
       <c r="F22" t="s">
         <v>8</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>44.6</v>
       </c>
@@ -1258,26 +884,8 @@
       <c r="F23" t="s">
         <v>6</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1651</v>
       </c>
@@ -1295,24 +903,6 @@
       </c>
       <c r="F24" t="s">
         <v>6</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>